<commit_message>
cleaned user data, combined user data with org ids and names
</commit_message>
<xml_diff>
--- a/scripts/org_list.xlsx
+++ b/scripts/org_list.xlsx
@@ -85,7 +85,7 @@
     <t>Allied Agent Office - aparna</t>
   </si>
   <si>
-    <t>Ardan's - aparna</t>
+    <t>Ardans - aparna</t>
   </si>
   <si>
     <t>Asian Fusion - aparna</t>
@@ -106,7 +106,7 @@
     <t>Blockbuster Music - aparna</t>
   </si>
   <si>
-    <t>Bob's super ford - aparna</t>
+    <t>Bobs super ford - aparna</t>
   </si>
   <si>
     <t>Bodega Club - aparna</t>
@@ -157,7 +157,7 @@
     <t>Eisner Food Stores2 - aparna</t>
   </si>
   <si>
-    <t>Erol's - aparna</t>
+    <t>Erols - aparna</t>
   </si>
   <si>
     <t>Express Logistics and Transport - aparna</t>
@@ -169,7 +169,7 @@
     <t>External ID Org - aparna</t>
   </si>
   <si>
-    <t>Farrell's Ice Cream Parlour - aparna</t>
+    <t>Farrells Ice Cream Parlour - aparna</t>
   </si>
   <si>
     <t>fast org - aparna</t>
@@ -193,7 +193,7 @@
     <t>Gold Medal - aparna</t>
   </si>
   <si>
-    <t>Grand Hotels &amp; Resorts Ltd - aparna</t>
+    <t>Grand Hotels  Resorts Ltd - aparna</t>
   </si>
   <si>
     <t>Grey Fade - aparna</t>
@@ -205,7 +205,7 @@
     <t>Helios Air - aparna</t>
   </si>
   <si>
-    <t>Herman's World of Sporting Goods - aparna</t>
+    <t>Hermans World of Sporting Goods - aparna</t>
   </si>
   <si>
     <t>Home Quarters Warehouse - aparna</t>
@@ -217,7 +217,7 @@
     <t>House Of Denmark - aparna</t>
   </si>
   <si>
-    <t>Hudson's MensWear - aparna</t>
+    <t>Hudsons MensWear - aparna</t>
   </si>
   <si>
     <t>Incluesiv - aparna</t>
@@ -265,10 +265,10 @@
     <t>Merrymaking2 - aparna</t>
   </si>
   <si>
-    <t>Mervyn's - aparna</t>
-  </si>
-  <si>
-    <t>Mighty Casey's - aparna</t>
+    <t>Mervyns - aparna</t>
+  </si>
+  <si>
+    <t>Mighty Caseys - aparna</t>
   </si>
   <si>
     <t>Monk Home Funding Services - aparna</t>
@@ -292,10 +292,10 @@
     <t>Northern Reflections - aparna</t>
   </si>
   <si>
-    <t>Odyssey Records &amp; Tapes - aparna</t>
-  </si>
-  <si>
-    <t>Ole's - aparna</t>
+    <t>Odyssey Records  Tapes - aparna</t>
+  </si>
+  <si>
+    <t>Oles - aparna</t>
   </si>
   <si>
     <t>Opticomp - aparna</t>
@@ -328,7 +328,7 @@
     <t>Sally SR Org - aparna</t>
   </si>
   <si>
-    <t>Sandy's - aparna</t>
+    <t>Sandys - aparna</t>
   </si>
   <si>
     <t>Seth Means Org - aparna</t>
@@ -352,7 +352,7 @@
     <t>Speedy org - aparna</t>
   </si>
   <si>
-    <t>Steve's Ice Cream - aparna</t>
+    <t>Steves Ice Cream - aparna</t>
   </si>
   <si>
     <t>Sunburst Garden Management - aparna</t>
@@ -379,16 +379,16 @@
     <t>Truckster Corp - aparna</t>
   </si>
   <si>
-    <t>Turtle's Records &amp; Tapes - aparna</t>
-  </si>
-  <si>
-    <t>United Oil &amp; Gas Corp. - aparna</t>
-  </si>
-  <si>
-    <t>United Oil &amp; Gas, Singapore - aparna</t>
-  </si>
-  <si>
-    <t>United Oil &amp; Gas, UK - aparna</t>
+    <t>Turtles Records  Tapes - aparna</t>
+  </si>
+  <si>
+    <t>United Oil  Gas Corp. - aparna</t>
+  </si>
+  <si>
+    <t>United Oil  Gas, Singapore - aparna</t>
+  </si>
+  <si>
+    <t>United Oil  Gas, UK - aparna</t>
   </si>
   <si>
     <t>University of Arizona - aparna</t>

</xml_diff>